<commit_message>
updated agent payment status
</commit_message>
<xml_diff>
--- a/backend/data/agents.xlsx
+++ b/backend/data/agents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hemanth\Development\Projects\EkluvyaCouponsTransactions\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068BE2F6-DF2F-4CB2-AD6D-AC8B9F3951C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C20652-4C76-47B1-B2FD-FD91FBBEEA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6669" uniqueCount="5440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6672" uniqueCount="5443">
   <si>
     <t>name</t>
   </si>
@@ -24902,6 +24902,15 @@
   </si>
   <si>
     <t>ASAN2606</t>
+  </si>
+  <si>
+    <t>SENSYS</t>
+  </si>
+  <si>
+    <t>DSEN7971</t>
+  </si>
+  <si>
+    <t>um@sensysindia.com</t>
   </si>
 </sst>
 </file>
@@ -25179,7 +25188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -25290,6 +25299,9 @@
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -25510,10 +25522,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1695"/>
+  <dimension ref="A1:Z1696"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1676" workbookViewId="0">
-      <selection activeCell="A1702" sqref="A1702"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H575" sqref="H575"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -54119,6 +54131,21 @@
       <c r="E1695" s="13" t="s">
         <v>3430</v>
       </c>
+    </row>
+    <row r="1696" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1696" s="37" t="s">
+        <v>5440</v>
+      </c>
+      <c r="B1696" s="9">
+        <v>9867307971</v>
+      </c>
+      <c r="C1696" s="10" t="s">
+        <v>5441</v>
+      </c>
+      <c r="D1696" s="38" t="s">
+        <v>5442</v>
+      </c>
+      <c r="E1696" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>